<commit_message>
add dependance IG NOS 1.2.0 ac5dd1e1e82f628859c2d904f4f01273a2b307b7
</commit_message>
<xml_diff>
--- a/sd-add-dependance-IG-NOS/ig/ValueSet-ror-usage-context-type-vs.xlsx
+++ b/sd-add-dependance-IG-NOS/ig/ValueSet-ror-usage-context-type-vs.xlsx
@@ -8,9 +8,9 @@
   <sheets>
     <sheet name="Metadata" r:id="rId3" sheetId="1"/>
     <sheet name="Include from UsageContextType" r:id="rId4" sheetId="2"/>
-    <sheet name="Include from TRE-R67-TypeStru" r:id="rId5" sheetId="3"/>
-    <sheet name="Include from TRE-R04-TypeSavo" r:id="rId6" sheetId="4"/>
-    <sheet name="Include from TRE-R288-TypePro" r:id="rId7" sheetId="5"/>
+    <sheet name="Include from TRE_R67-TypeStru" r:id="rId5" sheetId="3"/>
+    <sheet name="Include from TRE_R04-TypeSavo" r:id="rId6" sheetId="4"/>
+    <sheet name="Include from TRE_R288-TypePro" r:id="rId7" sheetId="5"/>
   </sheets>
 </workbook>
 </file>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-04-08T13:36:34+00:00</t>
+    <t>2024-04-08T14:06:04+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>